<commit_message>
Appropriate changes to skel files
</commit_message>
<xml_diff>
--- a/MotorCharacterization.xlsx
+++ b/MotorCharacterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayaat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cellulo_Thesis_Programming\robots_firmware\cellulo\tremo_foot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>count</t>
   </si>
@@ -33,6 +33,27 @@
   </si>
   <si>
     <t>pwm</t>
+  </si>
+  <si>
+    <t>old code speed</t>
+  </si>
+  <si>
+    <t>old code rpm count</t>
+  </si>
+  <si>
+    <t>new code speed</t>
+  </si>
+  <si>
+    <t>new code rpm count</t>
+  </si>
+  <si>
+    <t>volt</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>wihtout filter</t>
   </si>
 </sst>
 </file>
@@ -419,11 +440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162808016"/>
-        <c:axId val="162805840"/>
+        <c:axId val="1760883376"/>
+        <c:axId val="1760885008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162808016"/>
+        <c:axId val="1760883376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,12 +501,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162805840"/>
+        <c:crossAx val="1760885008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162805840"/>
+        <c:axId val="1760885008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162808016"/>
+        <c:crossAx val="1760883376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1151,16 +1172,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1445,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" activeCellId="1" sqref="C2:C9 A2:A9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,9 +1477,13 @@
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1469,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>247</v>
       </c>
@@ -1479,8 +1504,14 @@
       <c r="C2">
         <v>4356</v>
       </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>4.42</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>347</v>
       </c>
@@ -1490,8 +1521,14 @@
       <c r="C3">
         <v>5985</v>
       </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>447</v>
       </c>
@@ -1501,8 +1538,11 @@
       <c r="C4">
         <v>7436</v>
       </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>547</v>
       </c>
@@ -1512,8 +1552,20 @@
       <c r="C5">
         <v>9261</v>
       </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>647</v>
       </c>
@@ -1523,8 +1575,23 @@
       <c r="C6">
         <v>12399</v>
       </c>
+      <c r="I6">
+        <v>247</v>
+      </c>
+      <c r="J6">
+        <v>4320</v>
+      </c>
+      <c r="K6">
+        <v>4185</v>
+      </c>
+      <c r="L6">
+        <v>4320</v>
+      </c>
+      <c r="M6">
+        <v>4185</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>747</v>
       </c>
@@ -1534,8 +1601,17 @@
       <c r="C7">
         <v>13545</v>
       </c>
+      <c r="I7">
+        <v>347</v>
+      </c>
+      <c r="J7">
+        <v>5160</v>
+      </c>
+      <c r="K7">
+        <v>5054</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>847</v>
       </c>
@@ -1545,8 +1621,17 @@
       <c r="C8">
         <v>16607</v>
       </c>
+      <c r="I8">
+        <v>447</v>
+      </c>
+      <c r="J8">
+        <v>7380</v>
+      </c>
+      <c r="K8">
+        <v>7168</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>947</v>
       </c>
@@ -1555,6 +1640,41 @@
       </c>
       <c r="C9">
         <v>16606</v>
+      </c>
+      <c r="I9">
+        <v>547</v>
+      </c>
+      <c r="J9">
+        <v>9480</v>
+      </c>
+      <c r="K9">
+        <v>9536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>947</v>
+      </c>
+      <c r="J13">
+        <v>15660</v>
+      </c>
+      <c r="K13">
+        <v>14753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>